<commit_message>
Update Grupo 9 Acta seguimiento.xlsx
Actualizacion Acta
</commit_message>
<xml_diff>
--- a/Proyecto Ciclo 3/Grupo 9 Acta seguimiento.xlsx
+++ b/Proyecto Ciclo 3/Grupo 9 Acta seguimiento.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Fecha</t>
   </si>
@@ -197,12 +197,18 @@
   <si>
     <t>Se realiza verificacion del diagrama de clases de clases, queda pendiente la realizacion del diagrama E-R y quedo asignado el diagrama de casos de uso a Henry Martinez, se cambiar elformato del acta quedando aprobado por los integrantes, proxima reunion viernes 24 de Septiembre.</t>
   </si>
+  <si>
+    <t>10:40pm</t>
+  </si>
+  <si>
+    <t>Se realiza muestra de codificacion para Sripnt 3, se unifican ideas y se complementa el desarrollo y el cargue de la URL en la plataforma de mision TIC. Uso de CSS y boostrap.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +240,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -502,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -535,6 +549,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -562,11 +582,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1022,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1038,38 +1059,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="A1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:5" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="22" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="19"/>
+      <c r="E3" s="21"/>
     </row>
     <row r="4" spans="1:5" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
@@ -1143,25 +1164,35 @@
       <c r="A9" s="9">
         <v>44461</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="17" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="3"/>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="28">
+        <v>44467</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -1171,7 +1202,7 @@
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1834,7 +1865,7 @@
     <mergeCell ref="A1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>